<commit_message>
updated pa vs qp table
</commit_message>
<xml_diff>
--- a/HJA_scripts/08_reference_sequences_datasets/pa_vs_qp_tables_20210402.xlsx
+++ b/HJA_scripts/08_reference_sequences_datasets/pa_vs_qp_tables_20210402.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Luo_Mingjie_Oregon/HJA_analyses_Kelpie/HJA_scripts/08_reference_sequences_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E01B53-CF66-154E-96EE-BC59805EDC07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719921FE-1C56-7E46-AD6B-2D794C8393F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{53C8B974-4F2E-7B4E-B4C5-DAE879BD5093}"/>
   </bookViews>
@@ -726,24 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -752,6 +734,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12516,8 +12516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF64AE32-F5AF-E840-B10C-98CC4787FA60}">
   <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N13" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12560,26 +12560,26 @@
     <row r="2" spans="2:40" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="69"/>
+      <c r="J2" s="68"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="67" t="s">
+      <c r="S2" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
       <c r="W2" s="28"/>
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.2">
@@ -12600,8 +12600,8 @@
       <c r="H3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="68"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="R3" s="11"/>
@@ -12936,37 +12936,37 @@
       <c r="AN10" s="51"/>
     </row>
     <row r="11" spans="2:40" s="5" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="68" t="s">
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="65" t="s">
+      <c r="M11" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="S11" s="65" t="s">
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="S11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="Y11" s="70" t="s">
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
+      <c r="Y11" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="Z11" s="71"/>
-      <c r="AA11" s="71"/>
-      <c r="AB11" s="72"/>
+      <c r="Z11" s="65"/>
+      <c r="AA11" s="65"/>
+      <c r="AB11" s="66"/>
     </row>
     <row r="12" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D12" s="24" t="s">
@@ -12984,8 +12984,8 @@
       <c r="H12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="68"/>
-      <c r="J12" s="66"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="69"/>
       <c r="M12" s="24" t="s">
         <v>0</v>
       </c>
@@ -13435,19 +13435,19 @@
       <c r="AB20" s="42"/>
     </row>
     <row r="21" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="S21" s="65" t="s">
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="S21" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="T21" s="65"/>
-      <c r="U21" s="65"/>
-      <c r="V21" s="65"/>
-      <c r="W21" s="66" t="s">
+      <c r="T21" s="67"/>
+      <c r="U21" s="67"/>
+      <c r="V21" s="67"/>
+      <c r="W21" s="69" t="s">
         <v>32</v>
       </c>
       <c r="Y21" s="21" t="s">
@@ -13482,7 +13482,7 @@
       <c r="V22" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="W22" s="66"/>
+      <c r="W22" s="69"/>
       <c r="Y22" s="43" t="s">
         <v>49</v>
       </c>
@@ -13774,21 +13774,21 @@
     <row r="30" spans="1:28" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="65" t="s">
+      <c r="D30" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
       <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
@@ -13937,12 +13937,12 @@
       <c r="P36" s="11"/>
     </row>
     <row r="39" spans="3:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D40" s="24" t="s">
@@ -14041,6 +14041,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="Y11:AB11"/>
     <mergeCell ref="D39:G39"/>
     <mergeCell ref="M11:P11"/>
@@ -14050,13 +14057,6 @@
     <mergeCell ref="S21:V21"/>
     <mergeCell ref="S11:V11"/>
     <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>